<commit_message>
Updated text for latest simulation results
</commit_message>
<xml_diff>
--- a/data/methodcalls-vs-duration.xlsx
+++ b/data/methodcalls-vs-duration.xlsx
@@ -162,8 +162,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -220,7 +222,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -245,6 +247,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -269,6 +272,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,7 +605,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -874,8 +878,8 @@
         <f t="shared" si="2"/>
         <v>10428.456978624034</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
+      <c r="C25" t="str">
+        <f>C7</f>
         <v>CoreListJoinA.calc_func</v>
       </c>
     </row>

</xml_diff>